<commit_message>
probably, possibly, maybe finished CPU?
</commit_message>
<xml_diff>
--- a/documentation/notes/cpu-states.xlsx
+++ b/documentation/notes/cpu-states.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\UNI\FHDW\LogicWorks\logicworks-alu\documentation\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDBC7CE-7E4B-4162-90AB-9766992A5C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2965CDE6-E732-44B0-B18D-A9457AFE7056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" xr2:uid="{5EC45C85-F338-440C-92FA-DD2EC66A5570}"/>
+    <workbookView xWindow="-6070" yWindow="-21710" windowWidth="38620" windowHeight="21820" xr2:uid="{5EC45C85-F338-440C-92FA-DD2EC66A5570}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="78">
   <si>
     <t>Qn3</t>
   </si>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t>a~c~dg + bcf + cd + de + ~b~c + ~ac + ~ad</t>
+  </si>
+  <si>
+    <t>ANY OTHER</t>
   </si>
 </sst>
 </file>
@@ -633,14 +636,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AH115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
-    <col min="2" max="5" width="4.140625" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="9" width="7" customWidth="1"/>
     <col min="10" max="10" width="16.140625" customWidth="1"/>
@@ -660,7 +666,7 @@
     <col min="30" max="30" width="4.85546875" customWidth="1"/>
     <col min="31" max="31" width="9.85546875" customWidth="1"/>
     <col min="32" max="32" width="0.5703125" customWidth="1"/>
-    <col min="33" max="33" width="0.140625" customWidth="1"/>
+    <col min="33" max="33" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -864,12 +870,12 @@
         <v>1</v>
       </c>
       <c r="AG3" t="str">
-        <f>_xlfn.CONCAT(P3,IF(P3=1,"1111",_xlfn.CONCAT(Q3:T3)),U3:AE3)</f>
-        <v>1111100010101101</v>
+        <f>_xlfn.CONCAT(P3,IF(P3=1,IF(J3="x","0000","0001"),_xlfn.CONCAT(Q3:T3)),U3:AE3)</f>
+        <v>1000000010101101</v>
       </c>
       <c r="AH3" t="str">
-        <f>_xlfn.CONCAT(BIN2HEX(LEFT(AG3,4),1),BIN2HEX(RIGHT(AG3,8),2))</f>
-        <v>FAD</v>
+        <f>_xlfn.CONCAT(BIN2HEX(LEFT(AG3,8),2),BIN2HEX(RIGHT(AG3,8),2))</f>
+        <v>80AD</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
@@ -964,12 +970,12 @@
         <v>1</v>
       </c>
       <c r="AG4" t="str">
-        <f t="shared" ref="AG4:AG28" si="0">_xlfn.CONCAT(P4,IF(P4=1,"1111",_xlfn.CONCAT(Q4:T4)),U4:AE4)</f>
-        <v>1111100010101101</v>
+        <f t="shared" ref="AG4:AG29" si="0">_xlfn.CONCAT(P4,IF(P4=1,IF(J4="x","0000","0001"),_xlfn.CONCAT(Q4:T4)),U4:AE4)</f>
+        <v>1000000010101101</v>
       </c>
       <c r="AH4" t="str">
-        <f t="shared" ref="AH4:AH28" si="1">_xlfn.CONCAT(BIN2HEX(LEFT(AG4,4),1),BIN2HEX(RIGHT(AG4,8),2))</f>
-        <v>FAD</v>
+        <f t="shared" ref="AH4:AH29" si="1">_xlfn.CONCAT(BIN2HEX(LEFT(AG4,8),2),BIN2HEX(RIGHT(AG4,8),2))</f>
+        <v>80AD</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
@@ -1065,11 +1071,11 @@
       </c>
       <c r="AG5" t="str">
         <f t="shared" si="0"/>
-        <v>1111100010101101</v>
+        <v>1000000010101101</v>
       </c>
       <c r="AH5" t="str">
         <f t="shared" si="1"/>
-        <v>FAD</v>
+        <v>80AD</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
@@ -1165,11 +1171,11 @@
       </c>
       <c r="AG6" t="str">
         <f t="shared" si="0"/>
-        <v>1111100010101101</v>
+        <v>1000000010101101</v>
       </c>
       <c r="AH6" t="str">
         <f t="shared" si="1"/>
-        <v>FAD</v>
+        <v>80AD</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
@@ -1265,11 +1271,11 @@
       </c>
       <c r="AG7" t="str">
         <f t="shared" si="0"/>
-        <v>1111100010101101</v>
+        <v>1000000010101101</v>
       </c>
       <c r="AH7" t="str">
         <f t="shared" si="1"/>
-        <v>FAD</v>
+        <v>80AD</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
@@ -1365,11 +1371,11 @@
       </c>
       <c r="AG8" t="str">
         <f t="shared" si="0"/>
-        <v>1111100010101101</v>
+        <v>1000000010101101</v>
       </c>
       <c r="AH8" t="str">
         <f t="shared" si="1"/>
-        <v>FAD</v>
+        <v>80AD</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
@@ -1465,11 +1471,11 @@
       </c>
       <c r="AG9" t="str">
         <f t="shared" si="0"/>
-        <v>1111100010101101</v>
+        <v>1000000010101101</v>
       </c>
       <c r="AH9" t="str">
         <f t="shared" si="1"/>
-        <v>FAD</v>
+        <v>80AD</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
@@ -1565,11 +1571,11 @@
       </c>
       <c r="AG10" t="str">
         <f t="shared" si="0"/>
-        <v>1111100010101101</v>
+        <v>1000000010101101</v>
       </c>
       <c r="AH10" t="str">
         <f t="shared" si="1"/>
-        <v>FAD</v>
+        <v>80AD</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
@@ -1665,11 +1671,11 @@
       </c>
       <c r="AG11" t="str">
         <f t="shared" si="0"/>
-        <v>1111100010101101</v>
+        <v>1000000010101101</v>
       </c>
       <c r="AH11" t="str">
         <f t="shared" si="1"/>
-        <v>FAD</v>
+        <v>80AD</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
@@ -1765,11 +1771,11 @@
       </c>
       <c r="AG12" t="str">
         <f t="shared" si="0"/>
-        <v>1111100010101101</v>
+        <v>1000000010101101</v>
       </c>
       <c r="AH12" t="str">
         <f t="shared" si="1"/>
-        <v>FAD</v>
+        <v>80AD</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
@@ -1865,11 +1871,11 @@
       </c>
       <c r="AG13" t="str">
         <f t="shared" si="0"/>
-        <v>1111100010101101</v>
+        <v>1000000010101101</v>
       </c>
       <c r="AH13" t="str">
         <f t="shared" si="1"/>
-        <v>FAD</v>
+        <v>80AD</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
@@ -1965,21 +1971,21 @@
       </c>
       <c r="AG14" t="str">
         <f t="shared" si="0"/>
-        <v>1111100010101101</v>
+        <v>1000000010101101</v>
       </c>
       <c r="AH14" t="str">
         <f t="shared" si="1"/>
-        <v>FAD</v>
+        <v>80AD</v>
       </c>
     </row>
     <row r="15" spans="1:34" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AG15" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(P15,IF(P15=1,IF(J15="x","0000","0001"),_xlfn.CONCAT(Q15:T15)),U15:AE15)</f>
         <v/>
       </c>
       <c r="AH15" t="str">
-        <f t="shared" si="1"/>
-        <v>000</v>
+        <f>_xlfn.CONCAT(BIN2HEX(LEFT(AG15,8),2),BIN2HEX(RIGHT(AG15,8),2))</f>
+        <v>0000</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
@@ -2074,12 +2080,12 @@
         <v>1</v>
       </c>
       <c r="AG16" t="str">
-        <f>_xlfn.CONCAT(P16,IF(P16=1,"1111",_xlfn.CONCAT(Q16:T16)),U16:AE16)</f>
+        <f t="shared" si="0"/>
         <v>0000100010001101</v>
       </c>
       <c r="AH16" t="str">
         <f t="shared" si="1"/>
-        <v>08D</v>
+        <v>088D</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
@@ -2179,7 +2185,7 @@
       </c>
       <c r="AH17" t="str">
         <f t="shared" si="1"/>
-        <v>00D</v>
+        <v>010D</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
@@ -2279,7 +2285,7 @@
       </c>
       <c r="AH18" t="str">
         <f t="shared" si="1"/>
-        <v>2AD</v>
+        <v>22AD</v>
       </c>
     </row>
     <row r="19" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2375,11 +2381,11 @@
       </c>
       <c r="AG19" t="str">
         <f t="shared" si="0"/>
-        <v>1111110010101101</v>
+        <v>1000110010101101</v>
       </c>
       <c r="AH19" t="str">
         <f t="shared" si="1"/>
-        <v>FAD</v>
+        <v>8CAD</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
@@ -2475,11 +2481,11 @@
       </c>
       <c r="AG20" t="str">
         <f t="shared" si="0"/>
-        <v>1111110010101101</v>
+        <v>1000110010101101</v>
       </c>
       <c r="AH20" t="str">
         <f t="shared" si="1"/>
-        <v>FAD</v>
+        <v>8CAD</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
@@ -2579,7 +2585,7 @@
       </c>
       <c r="AH21" t="str">
         <f t="shared" si="1"/>
-        <v>04C</v>
+        <v>064C</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
@@ -2679,7 +2685,7 @@
       </c>
       <c r="AH22" t="str">
         <f t="shared" si="1"/>
-        <v>045</v>
+        <v>0645</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
@@ -2779,7 +2785,7 @@
       </c>
       <c r="AH23" t="str">
         <f t="shared" si="1"/>
-        <v>4AD</v>
+        <v>42AD</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
@@ -2879,7 +2885,7 @@
       </c>
       <c r="AH24" t="str">
         <f t="shared" si="1"/>
-        <v>4AD</v>
+        <v>4CAD</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
@@ -2979,7 +2985,7 @@
       </c>
       <c r="AH25" t="str">
         <f t="shared" si="1"/>
-        <v>02D</v>
+        <v>002D</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
@@ -3079,7 +3085,7 @@
       </c>
       <c r="AH26" t="str">
         <f t="shared" si="1"/>
-        <v>04D</v>
+        <v>064D</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
@@ -3179,7 +3185,7 @@
       </c>
       <c r="AH27" t="str">
         <f t="shared" si="1"/>
-        <v>04F</v>
+        <v>024F</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
@@ -3279,7 +3285,107 @@
       </c>
       <c r="AH28" t="str">
         <f t="shared" si="1"/>
-        <v>051</v>
+        <v>0251</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" t="s">
+        <v>28</v>
+      </c>
+      <c r="K29" t="s">
+        <v>28</v>
+      </c>
+      <c r="L29" t="s">
+        <v>28</v>
+      </c>
+      <c r="M29" t="s">
+        <v>28</v>
+      </c>
+      <c r="N29" t="s">
+        <v>28</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <v>1</v>
+      </c>
+      <c r="Y29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>0</v>
+      </c>
+      <c r="AA29">
+        <v>0</v>
+      </c>
+      <c r="AB29">
+        <v>1</v>
+      </c>
+      <c r="AC29">
+        <v>1</v>
+      </c>
+      <c r="AD29">
+        <v>0</v>
+      </c>
+      <c r="AE29">
+        <v>1</v>
+      </c>
+      <c r="AG29" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000010001101</v>
+      </c>
+      <c r="AH29" t="str">
+        <f t="shared" si="1"/>
+        <v>008D</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
@@ -3296,13 +3402,13 @@
         <v>8</v>
       </c>
       <c r="F56" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="G56" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="H56" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
@@ -3663,13 +3769,13 @@
         <v>8</v>
       </c>
       <c r="F72" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="G72" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="H72" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
@@ -4030,13 +4136,13 @@
         <v>8</v>
       </c>
       <c r="F87" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="G87" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="H87" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.25">
@@ -4400,13 +4506,13 @@
         <v>8</v>
       </c>
       <c r="F102" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="G102" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="H102" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="103" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
actually save changes in excel
</commit_message>
<xml_diff>
--- a/documentation/notes/cpu-states.xlsx
+++ b/documentation/notes/cpu-states.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\UNI\FHDW\LogicWorks\logicworks-alu\documentation\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2965CDE6-E732-44B0-B18D-A9457AFE7056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22F0A8D-4016-421E-BDF4-032985645106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6070" yWindow="-21710" windowWidth="38620" windowHeight="21820" xr2:uid="{5EC45C85-F338-440C-92FA-DD2EC66A5570}"/>
   </bookViews>
@@ -636,8 +636,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AH115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="K68" sqref="K68"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix RAM MUX transition. TODO: fix Jump states, flag evaluation
</commit_message>
<xml_diff>
--- a/documentation/notes/cpu-states.xlsx
+++ b/documentation/notes/cpu-states.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\UNI\FHDW\LogicWorks\logicworks-alu\documentation\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22F0A8D-4016-421E-BDF4-032985645106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA4B4AF-6EA4-4EB9-A839-0A1537D67D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6070" yWindow="-21710" windowWidth="38620" windowHeight="21820" xr2:uid="{5EC45C85-F338-440C-92FA-DD2EC66A5570}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" xr2:uid="{5EC45C85-F338-440C-92FA-DD2EC66A5570}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -636,8 +636,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AH115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2062,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="Z16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA16">
         <v>0</v>
@@ -2081,11 +2081,11 @@
       </c>
       <c r="AG16" t="str">
         <f t="shared" si="0"/>
-        <v>0000100010001101</v>
+        <v>0000100010101101</v>
       </c>
       <c r="AH16" t="str">
         <f t="shared" si="1"/>
-        <v>088D</v>
+        <v>08AD</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
@@ -2162,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="Z17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA17">
         <v>0</v>
@@ -2181,11 +2181,11 @@
       </c>
       <c r="AG17" t="str">
         <f t="shared" si="0"/>
-        <v>0000000100001101</v>
+        <v>0000000100101101</v>
       </c>
       <c r="AH17" t="str">
         <f t="shared" si="1"/>
-        <v>010D</v>
+        <v>012D</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
@@ -3062,7 +3062,7 @@
         <v>1</v>
       </c>
       <c r="Z26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA26">
         <v>0</v>
@@ -3081,11 +3081,11 @@
       </c>
       <c r="AG26" t="str">
         <f t="shared" si="0"/>
-        <v>0000011001001101</v>
+        <v>0000011001101101</v>
       </c>
       <c r="AH26" t="str">
         <f t="shared" si="1"/>
-        <v>064D</v>
+        <v>066D</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
@@ -3162,7 +3162,7 @@
         <v>1</v>
       </c>
       <c r="Z27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA27">
         <v>0</v>
@@ -3181,11 +3181,11 @@
       </c>
       <c r="AG27" t="str">
         <f t="shared" si="0"/>
-        <v>0000001001001111</v>
+        <v>0000001001101111</v>
       </c>
       <c r="AH27" t="str">
         <f t="shared" si="1"/>
-        <v>024F</v>
+        <v>026F</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
@@ -3262,7 +3262,7 @@
         <v>1</v>
       </c>
       <c r="Z28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA28">
         <v>1</v>
@@ -3281,11 +3281,11 @@
       </c>
       <c r="AG28" t="str">
         <f t="shared" si="0"/>
-        <v>0000001001010001</v>
+        <v>0000001001110001</v>
       </c>
       <c r="AH28" t="str">
         <f t="shared" si="1"/>
-        <v>0251</v>
+        <v>0271</v>
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
@@ -3362,7 +3362,7 @@
         <v>0</v>
       </c>
       <c r="Z29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA29">
         <v>0</v>
@@ -3381,11 +3381,11 @@
       </c>
       <c r="AG29" t="str">
         <f t="shared" si="0"/>
-        <v>0000000010001101</v>
+        <v>0000000010101101</v>
       </c>
       <c r="AH29" t="str">
         <f t="shared" si="1"/>
-        <v>008D</v>
+        <v>00AD</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated excel and yed files
</commit_message>
<xml_diff>
--- a/documentation/notes/cpu-states.xlsx
+++ b/documentation/notes/cpu-states.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\UNI\FHDW\LogicWorks\logicworks-alu\documentation\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8112CAD6-2DFE-47C0-88E9-4BD5655ACBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4530B5-A940-4ECD-A126-B9D78EF26F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10230" yWindow="8055" windowWidth="31065" windowHeight="10590" xr2:uid="{5EC45C85-F338-440C-92FA-DD2EC66A5570}"/>
+    <workbookView xWindow="-6070" yWindow="-21710" windowWidth="38620" windowHeight="21820" xr2:uid="{5EC45C85-F338-440C-92FA-DD2EC66A5570}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -262,11 +262,6 @@
     <t>~a~b~e</t>
   </si>
   <si>
-    <t>~ac + 
-~ad + 
-~a~b</t>
-  </si>
-  <si>
     <t>ac~d + 
 ab~c + 
 a~bc</t>
@@ -281,6 +276,12 @@
 a~c + 
 ~a~b + 
 d</t>
+  </si>
+  <si>
+    <t>~bc~d +
+~ac + 
+~ad + 
+~a~b</t>
   </si>
 </sst>
 </file>
@@ -644,8 +645,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AH53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32:H34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3348,16 +3349,16 @@
         <v>58</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix ALU op / SWAP dependency
</commit_message>
<xml_diff>
--- a/documentation/notes/cpu-states.xlsx
+++ b/documentation/notes/cpu-states.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\UNI\FHDW\LogicWorks\logicworks-alu\documentation\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4530B5-A940-4ECD-A126-B9D78EF26F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432AC1FD-2E04-4C3F-BC74-8026183DFCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6070" yWindow="-21710" windowWidth="38620" windowHeight="21820" xr2:uid="{5EC45C85-F338-440C-92FA-DD2EC66A5570}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="82">
   <si>
     <t>Qn3</t>
   </si>
@@ -282,13 +282,26 @@
 ~ac + 
 ~ad + 
 ~a~b</t>
+  </si>
+  <si>
+    <t>BusyOut</t>
+  </si>
+  <si>
+    <t>NOP -&gt; MOV_REGREG</t>
+  </si>
+  <si>
+    <t>bc + 
+a~c + 
+~be + 
+~a~b + 
+d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,13 +315,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -320,16 +345,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -643,10 +673,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5316B296-034F-458C-9C64-711BF7C55C5F}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AH53"/>
+  <dimension ref="A1:AH67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3016,19 +3046,19 @@
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" t="s">
-        <v>28</v>
-      </c>
-      <c r="E29" t="s">
-        <v>28</v>
+        <v>80</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
       </c>
       <c r="F29" t="s">
         <v>28</v>
@@ -3061,10 +3091,10 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S29">
         <v>0</v>
@@ -3076,7 +3106,7 @@
         <v>0</v>
       </c>
       <c r="V29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W29">
         <v>0</v>
@@ -3085,13 +3115,13 @@
         <v>1</v>
       </c>
       <c r="Y29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z29">
         <v>1</v>
       </c>
       <c r="AA29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB29">
         <v>1</v>
@@ -3107,94 +3137,168 @@
       </c>
       <c r="AG29" t="str">
         <f t="shared" si="0"/>
-        <v>0000000010101101</v>
+        <v>0110001011111101</v>
       </c>
       <c r="AH29" t="str">
         <f t="shared" si="1"/>
+        <v>62FD</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" t="s">
+        <v>28</v>
+      </c>
+      <c r="K30" t="s">
+        <v>28</v>
+      </c>
+      <c r="L30" t="s">
+        <v>28</v>
+      </c>
+      <c r="M30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N30" t="s">
+        <v>28</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <v>1</v>
+      </c>
+      <c r="Y30">
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <v>1</v>
+      </c>
+      <c r="AA30">
+        <v>0</v>
+      </c>
+      <c r="AB30">
+        <v>1</v>
+      </c>
+      <c r="AC30">
+        <v>1</v>
+      </c>
+      <c r="AD30">
+        <v>0</v>
+      </c>
+      <c r="AE30">
+        <v>1</v>
+      </c>
+      <c r="AG30" t="str">
+        <f>_xlfn.CONCAT(P30,IF(P30=1,_xlfn.SWITCH(_xlfn.CONCAT(B30:E30), "0000","0000","0100","0001", "0111", "0010"),_xlfn.CONCAT(Q30:T30)),U30:AE30)</f>
+        <v>0000000010101101</v>
+      </c>
+      <c r="AH30" t="str">
+        <f>_xlfn.CONCAT(BIN2HEX(LEFT(AG30,8),2),BIN2HEX(RIGHT(AG30,8),2))</f>
         <v>00AD</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>55</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>56</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>57</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>58</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
         <v>34</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>36</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F32" t="s">
         <v>37</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G32" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" t="s">
+        <v>70</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>28</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" t="s">
+        <v>15</v>
       </c>
       <c r="H33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3214,36 +3318,39 @@
         <v>28</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
       </c>
       <c r="E35" t="s">
         <v>28</v>
       </c>
-      <c r="F35" t="s">
-        <v>28</v>
+      <c r="F35">
+        <v>1</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H35" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3257,36 +3364,36 @@
         <v>1</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>28</v>
       </c>
       <c r="F36" t="s">
         <v>28</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37" t="s">
-        <v>28</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
       </c>
       <c r="F37" t="s">
         <v>28</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -3303,35 +3410,58 @@
         <v>28</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" t="s">
         <v>28</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>65</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>28</v>
-      </c>
-      <c r="E39" t="s">
-        <v>28</v>
-      </c>
-      <c r="F39" t="s">
-        <v>28</v>
-      </c>
-      <c r="G39">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40">
         <v>0</v>
       </c>
     </row>
@@ -3491,7 +3621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>1</v>
       </c>
@@ -3517,7 +3647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>1</v>
       </c>
@@ -3543,7 +3673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>1</v>
       </c>
@@ -3569,7 +3699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>1</v>
       </c>
@@ -3595,7 +3725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>1</v>
       </c>
@@ -3618,6 +3748,354 @@
         <v>0</v>
       </c>
       <c r="I53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D56" t="s">
+        <v>57</v>
+      </c>
+      <c r="E56" t="s">
+        <v>58</v>
+      </c>
+      <c r="F56" t="s">
+        <v>59</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" t="s">
+        <v>79</v>
+      </c>
+      <c r="G57" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" t="s">
+        <v>14</v>
+      </c>
+      <c r="I57" t="s">
+        <v>15</v>
+      </c>
+      <c r="J57" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>28</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>28</v>
+      </c>
+      <c r="D59" t="s">
+        <v>28</v>
+      </c>
+      <c r="E59" t="s">
+        <v>28</v>
+      </c>
+      <c r="F59" t="s">
+        <v>28</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60" t="s">
+        <v>28</v>
+      </c>
+      <c r="F60" t="s">
+        <v>28</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63" t="s">
+        <v>28</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64" t="s">
+        <v>28</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
+        <v>28</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66" t="s">
+        <v>28</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
+        <v>28</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finish documentation, fix CPU
</commit_message>
<xml_diff>
--- a/documentation/notes/cpu-states.xlsx
+++ b/documentation/notes/cpu-states.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\UNI\FHDW\LogicWorks\logicworks-alu\documentation\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432AC1FD-2E04-4C3F-BC74-8026183DFCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC450A6F-3ED0-4680-9341-72E88A68582A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6070" yWindow="-21710" windowWidth="38620" windowHeight="21820" xr2:uid="{5EC45C85-F338-440C-92FA-DD2EC66A5570}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="83">
   <si>
     <t>Qn3</t>
   </si>
@@ -270,12 +270,6 @@
     <t>(b^d) + 
 ~c + 
 ~a</t>
-  </si>
-  <si>
-    <t>bc + 
-a~c + 
-~a~b + 
-d</t>
   </si>
   <si>
     <t>~bc~d +
@@ -295,6 +289,12 @@
 ~be + 
 ~a~b + 
 d</t>
+  </si>
+  <si>
+    <t>Inst fetch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int </t>
   </si>
 </sst>
 </file>
@@ -675,8 +675,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AH67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3046,7 +3046,7 @@
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3286,7 +3286,7 @@
         <v>70</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="E33" t="s">
         <v>11</v>
@@ -3466,292 +3466,17 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" t="s">
-        <v>56</v>
-      </c>
-      <c r="D43" t="s">
-        <v>57</v>
-      </c>
-      <c r="E43" t="s">
-        <v>58</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" t="s">
-        <v>8</v>
-      </c>
-      <c r="F44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" t="s">
-        <v>15</v>
-      </c>
-      <c r="I44" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <v>0</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <v>1</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46" t="s">
-        <v>28</v>
-      </c>
-      <c r="D46" t="s">
-        <v>28</v>
-      </c>
-      <c r="E46" t="s">
-        <v>28</v>
-      </c>
-      <c r="F46">
-        <v>1</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <v>1</v>
-      </c>
-      <c r="I46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47" t="s">
-        <v>28</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>1</v>
-      </c>
-      <c r="I47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-      <c r="I48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-      <c r="F49">
-        <v>0</v>
-      </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
-      <c r="H49">
-        <v>1</v>
-      </c>
-      <c r="I49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-      <c r="G50">
-        <v>1</v>
-      </c>
-      <c r="H50">
-        <v>1</v>
-      </c>
-      <c r="I50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51">
-        <v>0</v>
-      </c>
-      <c r="G51">
-        <v>1</v>
-      </c>
-      <c r="H51">
-        <v>1</v>
-      </c>
-      <c r="I51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="G52">
-        <v>1</v>
-      </c>
-      <c r="H52">
-        <v>1</v>
-      </c>
-      <c r="I52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-      <c r="F53">
-        <v>0</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="I53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>55</v>
       </c>
@@ -3768,7 +3493,7 @@
         <v>59</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>75</v>
@@ -3777,10 +3502,10 @@
         <v>76</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>5</v>
       </c>
@@ -3794,7 +3519,7 @@
         <v>8</v>
       </c>
       <c r="F57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G57" t="s">
         <v>13</v>
@@ -3809,7 +3534,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>0</v>
       </c>
@@ -3838,7 +3563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>0</v>
       </c>
@@ -3867,7 +3592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>1</v>
       </c>
@@ -3896,7 +3621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>1</v>
       </c>
@@ -3925,7 +3650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>1</v>
       </c>
@@ -3954,7 +3679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>1</v>
       </c>
@@ -3983,7 +3708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>1</v>
       </c>

</xml_diff>